<commit_message>
the last file was not up-to-date.
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KIEN\Desktop\CODING\Term 2 Freshman\IT003\Report 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D8EA81-6742-4C76-8216-E79B50B7F012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540882AD-DBD3-48C1-B114-4F5E0BDE5C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{40438754-7C5C-443C-BB08-AD73FB229D49}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{40438754-7C5C-443C-BB08-AD73FB229D49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Line #</t>
   </si>
@@ -61,6 +61,24 @@
   </si>
   <si>
     <t>Time (microseconds)</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>AVG</t>
   </si>
 </sst>
 </file>
@@ -91,7 +109,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -145,11 +163,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -181,10 +225,13 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -318,39 +365,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$14:$M$23</c:f>
+              <c:f>Sheet1!$N$15:$N$24</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>504025.4</c:v>
+                  <c:v>320284.59999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>419148.2</c:v>
+                  <c:v>319944.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>543674</c:v>
+                  <c:v>447979.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>546395</c:v>
+                  <c:v>433776.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>521505</c:v>
+                  <c:v>427924.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>516864.2</c:v>
+                  <c:v>423410.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>535845.80000000005</c:v>
+                  <c:v>476111.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>514118.40000000002</c:v>
+                  <c:v>447571</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>535451.4</c:v>
+                  <c:v>430224.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>536359.4</c:v>
+                  <c:v>478714.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -390,39 +437,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$14:$N$23</c:f>
+              <c:f>Sheet1!$O$15:$O$24</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>44651.199999999997</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>38630.199999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39262.400000000001</c:v>
+                  <c:v>40050.800000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>165007.20000000001</c:v>
+                  <c:v>160214.20000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>165108.20000000001</c:v>
+                  <c:v>158591.20000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>166701</c:v>
+                  <c:v>156892</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>166813.79999999999</c:v>
+                  <c:v>158841</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>156615.4</c:v>
+                  <c:v>160325</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>162147.6</c:v>
+                  <c:v>157352</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>169716.2</c:v>
+                  <c:v>159571.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>160198.39999999999</c:v>
+                  <c:v>157407</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -462,39 +509,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$14:$O$23</c:f>
+              <c:f>Sheet1!$P$15:$P$24</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>284111.59999999998</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>292073.40000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>303735.40000000002</c:v>
+                  <c:v>291393.59999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>405716.4</c:v>
+                  <c:v>400881</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>409192.8</c:v>
+                  <c:v>392133</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>403860.4</c:v>
+                  <c:v>393719.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>390891.8</c:v>
+                  <c:v>390746.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>391896.8</c:v>
+                  <c:v>388768</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>388658.8</c:v>
+                  <c:v>385133</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>408977.2</c:v>
+                  <c:v>393380.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>399977.2</c:v>
+                  <c:v>389241.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -534,39 +581,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$14:$P$23</c:f>
+              <c:f>Sheet1!$Q$15:$Q$24</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>133444.6</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>116486.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>154301.79999999999</c:v>
+                  <c:v>86022</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>267580.79999999999</c:v>
+                  <c:v>231991.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>262336.40000000002</c:v>
+                  <c:v>222552</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>261131.6</c:v>
+                  <c:v>219446.39999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>254518.2</c:v>
+                  <c:v>226182</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>243401.60000000001</c:v>
+                  <c:v>224570.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>253121.4</c:v>
+                  <c:v>220667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>253599.6</c:v>
+                  <c:v>228973.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>252373</c:v>
+                  <c:v>233385.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1459,10 +1506,10 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1789,10 +1836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BE822A-6BFD-4A6C-8063-66387E4EDFA0}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14:P23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N15" sqref="N15:Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1810,15 +1857,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="G1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1833,12 +1889,12 @@
       <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="12"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="5"/>
-      <c r="M2" s="3"/>
+      <c r="M2" s="12"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
@@ -1849,46 +1905,46 @@
         <v>6</v>
       </c>
       <c r="B3" s="7">
-        <v>467508</v>
+        <v>323821</v>
       </c>
       <c r="C3" s="7">
-        <v>42254</v>
+        <v>38746</v>
       </c>
       <c r="D3" s="7">
-        <v>284087</v>
+        <v>287391</v>
       </c>
       <c r="E3" s="8">
-        <v>122792</v>
+        <v>114766</v>
       </c>
       <c r="G3" s="6">
         <v>1</v>
       </c>
       <c r="H3" s="7">
-        <v>503048</v>
+        <v>337261</v>
       </c>
       <c r="I3" s="7">
-        <v>43709</v>
+        <v>41504</v>
       </c>
       <c r="J3" s="7">
-        <v>274919</v>
+        <v>312797</v>
       </c>
       <c r="K3" s="8">
-        <v>120400</v>
+        <v>121572</v>
       </c>
       <c r="M3" s="6">
         <v>1</v>
       </c>
       <c r="N3" s="7">
-        <v>496244</v>
+        <v>315086</v>
       </c>
       <c r="O3" s="7">
-        <v>42194</v>
+        <v>36774</v>
       </c>
       <c r="P3" s="7">
-        <v>274706</v>
+        <v>294495</v>
       </c>
       <c r="Q3" s="8">
-        <v>133403</v>
+        <v>117107</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -1896,46 +1952,46 @@
         <v>5</v>
       </c>
       <c r="B4" s="9">
-        <v>420987</v>
+        <v>324867</v>
       </c>
       <c r="C4" s="9">
-        <v>40994</v>
+        <v>38794</v>
       </c>
       <c r="D4" s="9">
-        <v>281739</v>
+        <v>284654</v>
       </c>
       <c r="E4" s="10">
-        <v>144680</v>
+        <v>82151</v>
       </c>
       <c r="G4" s="3">
         <v>2</v>
       </c>
       <c r="H4" s="9">
-        <v>408010</v>
+        <v>345466</v>
       </c>
       <c r="I4" s="9">
-        <v>39816</v>
+        <v>47043</v>
       </c>
       <c r="J4" s="9">
-        <v>282991</v>
+        <v>326374</v>
       </c>
       <c r="K4" s="10">
-        <v>149642</v>
+        <v>95340</v>
       </c>
       <c r="M4" s="3">
         <v>2</v>
       </c>
       <c r="N4" s="9">
-        <v>407726</v>
+        <v>310731</v>
       </c>
       <c r="O4" s="9">
-        <v>39769</v>
+        <v>37803</v>
       </c>
       <c r="P4" s="9">
-        <v>283314</v>
+        <v>284892</v>
       </c>
       <c r="Q4" s="10">
-        <v>160510</v>
+        <v>82422</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -1943,46 +1999,46 @@
         <v>3</v>
       </c>
       <c r="B5" s="7">
-        <v>532998</v>
+        <v>471272</v>
       </c>
       <c r="C5" s="7">
-        <v>151433</v>
+        <v>176610</v>
       </c>
       <c r="D5" s="7">
-        <v>390121</v>
+        <v>413281</v>
       </c>
       <c r="E5" s="8">
-        <v>254231</v>
+        <v>237119</v>
       </c>
       <c r="G5" s="6">
         <v>3</v>
       </c>
       <c r="H5" s="7">
-        <v>520977</v>
+        <v>478890</v>
       </c>
       <c r="I5" s="7">
-        <v>151147</v>
+        <v>166285</v>
       </c>
       <c r="J5" s="7">
-        <v>386219</v>
+        <v>421838</v>
       </c>
       <c r="K5" s="8">
-        <v>254242</v>
+        <v>231878</v>
       </c>
       <c r="M5" s="6">
         <v>3</v>
       </c>
       <c r="N5" s="7">
-        <v>510403</v>
+        <v>419954</v>
       </c>
       <c r="O5" s="7">
-        <v>158574</v>
+        <v>151296</v>
       </c>
       <c r="P5" s="7">
-        <v>377537</v>
+        <v>399477</v>
       </c>
       <c r="Q5" s="8">
-        <v>244108</v>
+        <v>236272</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -1990,46 +2046,46 @@
         <v>4</v>
       </c>
       <c r="B6" s="9">
-        <v>542836</v>
+        <v>455803</v>
       </c>
       <c r="C6" s="9">
-        <v>158913</v>
+        <v>168134</v>
       </c>
       <c r="D6" s="9">
-        <v>397016</v>
+        <v>418490</v>
       </c>
       <c r="E6" s="10">
-        <v>238781</v>
+        <v>231039</v>
       </c>
       <c r="G6" s="3">
         <v>4</v>
       </c>
       <c r="H6" s="9">
-        <v>496664</v>
+        <v>419574</v>
       </c>
       <c r="I6" s="9">
-        <v>154201</v>
+        <v>155759</v>
       </c>
       <c r="J6" s="9">
-        <v>368562</v>
+        <v>380571</v>
       </c>
       <c r="K6" s="10">
-        <v>240724</v>
+        <v>217613</v>
       </c>
       <c r="M6" s="3">
         <v>4</v>
       </c>
       <c r="N6" s="9">
-        <v>513072</v>
+        <v>425572</v>
       </c>
       <c r="O6" s="9">
-        <v>162077</v>
+        <v>158504</v>
       </c>
       <c r="P6" s="9">
-        <v>384989</v>
+        <v>388946</v>
       </c>
       <c r="Q6" s="10">
-        <v>238451</v>
+        <v>219894</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -2037,46 +2093,46 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>516261</v>
+        <v>439433</v>
       </c>
       <c r="C7" s="7">
-        <v>164142</v>
+        <v>165671</v>
       </c>
       <c r="D7" s="7">
-        <v>392144</v>
+        <v>429986</v>
       </c>
       <c r="E7" s="8">
-        <v>242557</v>
+        <v>224011</v>
       </c>
       <c r="G7" s="6">
         <v>5</v>
       </c>
       <c r="H7" s="7">
-        <v>491412</v>
+        <v>422216</v>
       </c>
       <c r="I7" s="7">
-        <v>154512</v>
+        <v>152458</v>
       </c>
       <c r="J7" s="7">
-        <v>389118</v>
+        <v>375841</v>
       </c>
       <c r="K7" s="8">
-        <v>245495</v>
+        <v>219844</v>
       </c>
       <c r="M7" s="6">
         <v>5</v>
       </c>
       <c r="N7" s="7">
-        <v>480752</v>
+        <v>412669</v>
       </c>
       <c r="O7" s="7">
-        <v>151069</v>
+        <v>157151</v>
       </c>
       <c r="P7" s="7">
-        <v>366645</v>
+        <v>394332</v>
       </c>
       <c r="Q7" s="8">
-        <v>235210</v>
+        <v>216743</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -2084,46 +2140,46 @@
         <v>6</v>
       </c>
       <c r="B8" s="9">
-        <v>514674</v>
+        <v>425221</v>
       </c>
       <c r="C8" s="9">
-        <v>153077</v>
+        <v>171910</v>
       </c>
       <c r="D8" s="9">
-        <v>370422</v>
+        <v>412363</v>
       </c>
       <c r="E8" s="10">
-        <v>243922</v>
+        <v>263965</v>
       </c>
       <c r="G8" s="3">
         <v>6</v>
       </c>
       <c r="H8" s="9">
-        <v>489632</v>
+        <v>415862</v>
       </c>
       <c r="I8" s="9">
-        <v>154744</v>
+        <v>153928</v>
       </c>
       <c r="J8" s="9">
-        <v>369308</v>
+        <v>378165</v>
       </c>
       <c r="K8" s="10">
-        <v>236101</v>
+        <v>219129</v>
       </c>
       <c r="M8" s="3">
         <v>6</v>
       </c>
       <c r="N8" s="9">
-        <v>484466</v>
+        <v>420468</v>
       </c>
       <c r="O8" s="9">
-        <v>152940</v>
+        <v>154794</v>
       </c>
       <c r="P8" s="9">
-        <v>371793</v>
+        <v>386424</v>
       </c>
       <c r="Q8" s="10">
-        <v>233858</v>
+        <v>212415</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -2131,46 +2187,46 @@
         <v>7</v>
       </c>
       <c r="B9" s="7">
-        <v>508597</v>
+        <v>674067</v>
       </c>
       <c r="C9" s="7">
-        <v>156965</v>
+        <v>177441</v>
       </c>
       <c r="D9" s="7">
-        <v>387301</v>
+        <v>401970</v>
       </c>
       <c r="E9" s="8">
-        <v>252348</v>
+        <v>229417</v>
       </c>
       <c r="G9" s="6">
         <v>7</v>
       </c>
       <c r="H9" s="7">
-        <v>497513</v>
+        <v>428674</v>
       </c>
       <c r="I9" s="7">
-        <v>153447</v>
+        <v>158103</v>
       </c>
       <c r="J9" s="7">
-        <v>369265</v>
+        <v>377420</v>
       </c>
       <c r="K9" s="8">
-        <v>237412</v>
+        <v>222492</v>
       </c>
       <c r="M9" s="6">
         <v>7</v>
       </c>
       <c r="N9" s="7">
-        <v>485730</v>
+        <v>413590</v>
       </c>
       <c r="O9" s="7">
-        <v>150888</v>
+        <v>153838</v>
       </c>
       <c r="P9" s="7">
-        <v>369147</v>
+        <v>395159</v>
       </c>
       <c r="Q9" s="8">
-        <v>234972</v>
+        <v>229432</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -2178,46 +2234,46 @@
         <v>8</v>
       </c>
       <c r="B10" s="9">
-        <v>493871</v>
+        <v>421649</v>
       </c>
       <c r="C10" s="9">
-        <v>155960</v>
+        <v>161438</v>
       </c>
       <c r="D10" s="9">
-        <v>371254</v>
+        <v>375478</v>
       </c>
       <c r="E10" s="10">
-        <v>238421</v>
+        <v>214954</v>
       </c>
       <c r="G10" s="3">
         <v>8</v>
       </c>
       <c r="H10" s="9">
-        <v>486761</v>
+        <v>453228</v>
       </c>
       <c r="I10" s="9">
-        <v>150723</v>
+        <v>155179</v>
       </c>
       <c r="J10" s="9">
-        <v>364819</v>
+        <v>385249</v>
       </c>
       <c r="K10" s="10">
-        <v>237463</v>
+        <v>224390</v>
       </c>
       <c r="M10" s="3">
         <v>8</v>
       </c>
       <c r="N10" s="9">
-        <v>481725</v>
+        <v>450998</v>
       </c>
       <c r="O10" s="9">
-        <v>157895</v>
+        <v>156717</v>
       </c>
       <c r="P10" s="9">
-        <v>364073</v>
+        <v>390354</v>
       </c>
       <c r="Q10" s="10">
-        <v>237661</v>
+        <v>218865</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -2225,46 +2281,46 @@
         <v>9</v>
       </c>
       <c r="B11" s="7">
-        <v>501064</v>
+        <v>459806</v>
       </c>
       <c r="C11" s="7">
-        <v>153706</v>
+        <v>171341</v>
       </c>
       <c r="D11" s="7">
-        <v>378360</v>
+        <v>420032</v>
       </c>
       <c r="E11" s="8">
-        <v>252245</v>
+        <v>266765</v>
       </c>
       <c r="G11" s="6">
         <v>9</v>
       </c>
       <c r="H11" s="7">
-        <v>501271</v>
+        <v>410000</v>
       </c>
       <c r="I11" s="7">
-        <v>151312</v>
+        <v>163753</v>
       </c>
       <c r="J11" s="7">
-        <v>370873</v>
+        <v>388287</v>
       </c>
       <c r="K11" s="8">
-        <v>238835</v>
+        <v>226688</v>
       </c>
       <c r="M11" s="6">
         <v>9</v>
       </c>
       <c r="N11" s="7">
-        <v>496126</v>
+        <v>410346</v>
       </c>
       <c r="O11" s="7">
-        <v>151836</v>
+        <v>154452</v>
       </c>
       <c r="P11" s="7">
-        <v>375589</v>
+        <v>388481</v>
       </c>
       <c r="Q11" s="8">
-        <v>235455</v>
+        <v>213470</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -2272,46 +2328,46 @@
         <v>10</v>
       </c>
       <c r="B12" s="9">
-        <v>516031</v>
+        <v>682415</v>
       </c>
       <c r="C12" s="9">
-        <v>154607</v>
+        <v>167114</v>
       </c>
       <c r="D12" s="9">
-        <v>371518</v>
+        <v>405027</v>
       </c>
       <c r="E12" s="10">
-        <v>240304</v>
+        <v>294897</v>
       </c>
       <c r="G12" s="3">
         <v>10</v>
       </c>
       <c r="H12" s="9">
-        <v>491396</v>
+        <v>444094</v>
       </c>
       <c r="I12" s="9">
-        <v>151446</v>
+        <v>155144</v>
       </c>
       <c r="J12" s="9">
-        <v>368450</v>
+        <v>385645</v>
       </c>
       <c r="K12" s="10">
-        <v>239331</v>
+        <v>223494</v>
       </c>
       <c r="M12" s="3">
         <v>10</v>
       </c>
       <c r="N12" s="9">
-        <v>479921</v>
+        <v>415208</v>
       </c>
       <c r="O12" s="9">
-        <v>152234</v>
+        <v>151740</v>
       </c>
       <c r="P12" s="9">
-        <v>363974</v>
+        <v>398367</v>
       </c>
       <c r="Q12" s="10">
-        <v>235871</v>
+        <v>214289</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -2322,483 +2378,524 @@
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4">
-        <v>567349</v>
-      </c>
-      <c r="C14" s="4">
-        <v>53115</v>
-      </c>
-      <c r="D14" s="4">
-        <v>314677</v>
-      </c>
-      <c r="E14" s="5">
-        <v>165926</v>
-      </c>
-      <c r="G14" s="3">
-        <v>1</v>
-      </c>
-      <c r="H14" s="4">
-        <v>485978</v>
-      </c>
-      <c r="I14" s="4">
-        <v>41984</v>
-      </c>
-      <c r="J14" s="4">
-        <v>272169</v>
-      </c>
-      <c r="K14" s="5">
-        <v>124702</v>
-      </c>
-      <c r="M14" s="11">
-        <f>AVERAGE(B3,H3,N3,B14,H14)</f>
-        <v>504025.4</v>
-      </c>
-      <c r="N14" s="11">
-        <f t="shared" ref="N14:P23" si="0">AVERAGE(C3,I3,O3,C14,I14)</f>
-        <v>44651.199999999997</v>
-      </c>
-      <c r="O14" s="11">
-        <f t="shared" si="0"/>
-        <v>284111.59999999998</v>
-      </c>
-      <c r="P14" s="11">
-        <f>AVERAGE(E3,K3,Q3,E14,K14)</f>
-        <v>133444.6</v>
+      <c r="A14" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
-        <v>2</v>
-      </c>
-      <c r="B15" s="7">
-        <v>462311</v>
-      </c>
-      <c r="C15" s="7">
-        <v>38162</v>
-      </c>
-      <c r="D15" s="7">
-        <v>371890</v>
-      </c>
-      <c r="E15" s="8">
-        <v>164193</v>
-      </c>
-      <c r="G15" s="6">
-        <v>2</v>
-      </c>
-      <c r="H15" s="7">
-        <v>396707</v>
-      </c>
-      <c r="I15" s="7">
-        <v>37571</v>
-      </c>
-      <c r="J15" s="7">
-        <v>298743</v>
-      </c>
-      <c r="K15" s="8">
-        <v>152484</v>
-      </c>
-      <c r="M15" s="11">
-        <f t="shared" ref="M15:M23" si="1">AVERAGE(B4,H4,N4,B15,H15)</f>
-        <v>419148.2</v>
-      </c>
-      <c r="N15" s="11">
-        <f t="shared" si="0"/>
-        <v>39262.400000000001</v>
-      </c>
-      <c r="O15" s="11">
-        <f t="shared" si="0"/>
-        <v>303735.40000000002</v>
-      </c>
-      <c r="P15" s="11">
-        <f>AVERAGE(E4,K4,Q4,E15,K15)</f>
-        <v>154301.79999999999</v>
+      <c r="A15" s="12">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4">
+        <v>315355</v>
+      </c>
+      <c r="C15" s="4">
+        <v>38507</v>
+      </c>
+      <c r="D15" s="4">
+        <v>281407</v>
+      </c>
+      <c r="E15" s="5">
+        <v>112738</v>
+      </c>
+      <c r="G15" s="12">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
+        <v>309900</v>
+      </c>
+      <c r="I15" s="4">
+        <v>37620</v>
+      </c>
+      <c r="J15" s="4">
+        <v>284277</v>
+      </c>
+      <c r="K15" s="5">
+        <v>116250</v>
+      </c>
+      <c r="M15" s="12">
+        <v>1</v>
+      </c>
+      <c r="N15" s="9">
+        <f>AVERAGE(B3,H3,N3,B15,H15)</f>
+        <v>320284.59999999998</v>
+      </c>
+      <c r="O15" s="4">
+        <f>AVERAGE(C3,I3,O3,C15,I15)</f>
+        <v>38630.199999999997</v>
+      </c>
+      <c r="P15" s="4">
+        <f>AVERAGE(D3,J3,P3,D15,J15)</f>
+        <v>292073.40000000002</v>
+      </c>
+      <c r="Q15" s="5">
+        <f>AVERAGE(E3,K3,Q3,E15,K15)</f>
+        <v>116486.6</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="A16" s="6">
+        <v>2</v>
+      </c>
+      <c r="B16" s="7">
+        <v>311435</v>
+      </c>
+      <c r="C16" s="7">
+        <v>39245</v>
+      </c>
+      <c r="D16" s="7">
+        <v>285957</v>
+      </c>
+      <c r="E16" s="8">
+        <v>85742</v>
+      </c>
+      <c r="G16" s="6">
+        <v>2</v>
+      </c>
+      <c r="H16" s="7">
+        <v>307225</v>
+      </c>
+      <c r="I16" s="7">
+        <v>37369</v>
+      </c>
+      <c r="J16" s="7">
+        <v>275091</v>
+      </c>
+      <c r="K16" s="8">
+        <v>84455</v>
+      </c>
+      <c r="M16" s="6">
+        <v>2</v>
+      </c>
+      <c r="N16" s="7">
+        <f>AVERAGE(B4,H4,N4,B16,H16)</f>
+        <v>319944.8</v>
+      </c>
+      <c r="O16" s="7">
+        <f>AVERAGE(C4,I4,O4,C16,I16)</f>
+        <v>40050.800000000003</v>
+      </c>
+      <c r="P16" s="7">
+        <f>AVERAGE(D4,J4,P4,D16,J16)</f>
+        <v>291393.59999999998</v>
+      </c>
+      <c r="Q16" s="8">
+        <f>AVERAGE(E4,K4,Q4,E16,K16)</f>
+        <v>86022</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
         <v>3</v>
       </c>
-      <c r="B16" s="9">
-        <v>631050</v>
-      </c>
-      <c r="C16" s="9">
-        <v>211253</v>
-      </c>
-      <c r="D16" s="9">
-        <v>504720</v>
-      </c>
-      <c r="E16" s="10">
-        <v>343417</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="B17" s="9">
+        <v>449618</v>
+      </c>
+      <c r="C17" s="9">
+        <v>155725</v>
+      </c>
+      <c r="D17" s="9">
+        <v>391491</v>
+      </c>
+      <c r="E17" s="10">
+        <v>228839</v>
+      </c>
+      <c r="G17" s="3">
         <v>3</v>
       </c>
-      <c r="H16" s="9">
-        <v>522942</v>
-      </c>
-      <c r="I16" s="9">
-        <v>152629</v>
-      </c>
-      <c r="J16" s="9">
-        <v>369985</v>
-      </c>
-      <c r="K16" s="10">
-        <v>241906</v>
-      </c>
-      <c r="M16" s="11">
-        <f t="shared" si="1"/>
-        <v>543674</v>
-      </c>
-      <c r="N16" s="11">
-        <f t="shared" si="0"/>
-        <v>165007.20000000001</v>
-      </c>
-      <c r="O16" s="11">
-        <f t="shared" si="0"/>
-        <v>405716.4</v>
-      </c>
-      <c r="P16" s="11">
-        <f t="shared" si="0"/>
-        <v>267580.79999999999</v>
+      <c r="H17" s="9">
+        <v>420165</v>
+      </c>
+      <c r="I17" s="9">
+        <v>151155</v>
+      </c>
+      <c r="J17" s="9">
+        <v>378318</v>
+      </c>
+      <c r="K17" s="10">
+        <v>225849</v>
+      </c>
+      <c r="M17" s="3">
+        <v>3</v>
+      </c>
+      <c r="N17" s="9">
+        <f>AVERAGE(B5,H5,N5,B17,H17)</f>
+        <v>447979.8</v>
+      </c>
+      <c r="O17" s="9">
+        <f>AVERAGE(C5,I5,O5,C17,I17)</f>
+        <v>160214.20000000001</v>
+      </c>
+      <c r="P17" s="9">
+        <f>AVERAGE(D5,J5,P5,D17,J17)</f>
+        <v>400881</v>
+      </c>
+      <c r="Q17" s="10">
+        <f>AVERAGE(E5,K5,Q5,E17,K17)</f>
+        <v>231991.4</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
         <v>4</v>
       </c>
-      <c r="B17" s="7">
-        <v>679109</v>
-      </c>
-      <c r="C17" s="7">
-        <v>184427</v>
-      </c>
-      <c r="D17" s="7">
-        <v>502313</v>
-      </c>
-      <c r="E17" s="8">
-        <v>350988</v>
-      </c>
-      <c r="G17" s="6">
+      <c r="B18" s="7">
+        <v>443654</v>
+      </c>
+      <c r="C18" s="7">
+        <v>159293</v>
+      </c>
+      <c r="D18" s="7">
+        <v>391536</v>
+      </c>
+      <c r="E18" s="8">
+        <v>223760</v>
+      </c>
+      <c r="G18" s="6">
         <v>4</v>
       </c>
-      <c r="H17" s="7">
-        <v>500294</v>
-      </c>
-      <c r="I17" s="7">
-        <v>165923</v>
-      </c>
-      <c r="J17" s="7">
-        <v>393084</v>
-      </c>
-      <c r="K17" s="8">
-        <v>242738</v>
-      </c>
-      <c r="M17" s="11">
-        <f t="shared" si="1"/>
-        <v>546395</v>
-      </c>
-      <c r="N17" s="11">
-        <f t="shared" si="0"/>
-        <v>165108.20000000001</v>
-      </c>
-      <c r="O17" s="11">
-        <f t="shared" si="0"/>
-        <v>409192.8</v>
-      </c>
-      <c r="P17" s="11">
-        <f t="shared" si="0"/>
-        <v>262336.40000000002</v>
+      <c r="H18" s="7">
+        <v>424281</v>
+      </c>
+      <c r="I18" s="7">
+        <v>151266</v>
+      </c>
+      <c r="J18" s="7">
+        <v>381122</v>
+      </c>
+      <c r="K18" s="8">
+        <v>220454</v>
+      </c>
+      <c r="M18" s="6">
+        <v>4</v>
+      </c>
+      <c r="N18" s="7">
+        <f>AVERAGE(B6,H6,N6,B18,H18)</f>
+        <v>433776.8</v>
+      </c>
+      <c r="O18" s="7">
+        <f>AVERAGE(C6,I6,O6,C18,I18)</f>
+        <v>158591.20000000001</v>
+      </c>
+      <c r="P18" s="7">
+        <f>AVERAGE(D6,J6,P6,D18,J18)</f>
+        <v>392133</v>
+      </c>
+      <c r="Q18" s="8">
+        <f>AVERAGE(E6,K6,Q6,E18,K18)</f>
+        <v>222552</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
         <v>5</v>
       </c>
-      <c r="B18" s="9">
-        <v>596059</v>
-      </c>
-      <c r="C18" s="9">
-        <v>209649</v>
-      </c>
-      <c r="D18" s="9">
-        <v>499823</v>
-      </c>
-      <c r="E18" s="10">
-        <v>346839</v>
-      </c>
-      <c r="G18" s="3">
+      <c r="B19" s="9">
+        <v>445648</v>
+      </c>
+      <c r="C19" s="9">
+        <v>156620</v>
+      </c>
+      <c r="D19" s="9">
+        <v>387477</v>
+      </c>
+      <c r="E19" s="10">
+        <v>220946</v>
+      </c>
+      <c r="G19" s="3">
         <v>5</v>
       </c>
-      <c r="H18" s="9">
-        <v>523041</v>
-      </c>
-      <c r="I18" s="9">
-        <v>154133</v>
-      </c>
-      <c r="J18" s="9">
-        <v>371572</v>
-      </c>
-      <c r="K18" s="10">
-        <v>235557</v>
-      </c>
-      <c r="M18" s="11">
-        <f t="shared" si="1"/>
-        <v>521505</v>
-      </c>
-      <c r="N18" s="11">
-        <f t="shared" si="0"/>
-        <v>166701</v>
-      </c>
-      <c r="O18" s="11">
-        <f t="shared" si="0"/>
-        <v>403860.4</v>
-      </c>
-      <c r="P18" s="11">
-        <f t="shared" si="0"/>
-        <v>261131.6</v>
+      <c r="H19" s="9">
+        <v>419656</v>
+      </c>
+      <c r="I19" s="9">
+        <v>152560</v>
+      </c>
+      <c r="J19" s="9">
+        <v>380960</v>
+      </c>
+      <c r="K19" s="10">
+        <v>215688</v>
+      </c>
+      <c r="M19" s="3">
+        <v>5</v>
+      </c>
+      <c r="N19" s="9">
+        <f>AVERAGE(B7,H7,N7,B19,H19)</f>
+        <v>427924.4</v>
+      </c>
+      <c r="O19" s="9">
+        <f>AVERAGE(C7,I7,O7,C19,I19)</f>
+        <v>156892</v>
+      </c>
+      <c r="P19" s="9">
+        <f>AVERAGE(D7,J7,P7,D19,J19)</f>
+        <v>393719.2</v>
+      </c>
+      <c r="Q19" s="10">
+        <f>AVERAGE(E7,K7,Q7,E19,K19)</f>
+        <v>219446.39999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="6">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
         <v>6</v>
       </c>
-      <c r="B19" s="7">
-        <v>599527</v>
-      </c>
-      <c r="C19" s="7">
-        <v>212196</v>
-      </c>
-      <c r="D19" s="7">
-        <v>459293</v>
-      </c>
-      <c r="E19" s="8">
-        <v>318545</v>
-      </c>
-      <c r="G19" s="6">
+      <c r="B20" s="7">
+        <v>440128</v>
+      </c>
+      <c r="C20" s="7">
+        <v>159196</v>
+      </c>
+      <c r="D20" s="7">
+        <v>399037</v>
+      </c>
+      <c r="E20" s="8">
+        <v>218224</v>
+      </c>
+      <c r="G20" s="6">
         <v>6</v>
       </c>
-      <c r="H19" s="7">
-        <v>496022</v>
-      </c>
-      <c r="I19" s="7">
-        <v>161112</v>
-      </c>
-      <c r="J19" s="7">
-        <v>383643</v>
-      </c>
-      <c r="K19" s="8">
-        <v>240165</v>
-      </c>
-      <c r="M19" s="11">
-        <f t="shared" si="1"/>
-        <v>516864.2</v>
-      </c>
-      <c r="N19" s="11">
-        <f t="shared" si="0"/>
-        <v>166813.79999999999</v>
-      </c>
-      <c r="O19" s="11">
-        <f t="shared" si="0"/>
-        <v>390891.8</v>
-      </c>
-      <c r="P19" s="11">
-        <f t="shared" si="0"/>
-        <v>254518.2</v>
+      <c r="H20" s="7">
+        <v>415374</v>
+      </c>
+      <c r="I20" s="7">
+        <v>154377</v>
+      </c>
+      <c r="J20" s="7">
+        <v>377745</v>
+      </c>
+      <c r="K20" s="8">
+        <v>217177</v>
+      </c>
+      <c r="M20" s="6">
+        <v>6</v>
+      </c>
+      <c r="N20" s="7">
+        <f>AVERAGE(B8,H8,N8,B20,H20)</f>
+        <v>423410.6</v>
+      </c>
+      <c r="O20" s="7">
+        <f>AVERAGE(C8,I8,O8,C20,I20)</f>
+        <v>158841</v>
+      </c>
+      <c r="P20" s="7">
+        <f>AVERAGE(D8,J8,P8,D20,J20)</f>
+        <v>390746.8</v>
+      </c>
+      <c r="Q20" s="8">
+        <f>AVERAGE(E8,K8,Q8,E20,K20)</f>
+        <v>226182</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>7</v>
       </c>
-      <c r="B20" s="9">
-        <v>691377</v>
-      </c>
-      <c r="C20" s="9">
-        <v>171535</v>
-      </c>
-      <c r="D20" s="9">
-        <v>463703</v>
-      </c>
-      <c r="E20" s="10">
-        <v>254639</v>
-      </c>
-      <c r="G20" s="3">
+      <c r="B21" s="9">
+        <v>444617</v>
+      </c>
+      <c r="C21" s="9">
+        <v>157465</v>
+      </c>
+      <c r="D21" s="9">
+        <v>389299</v>
+      </c>
+      <c r="E21" s="10">
+        <v>221247</v>
+      </c>
+      <c r="G21" s="3">
         <v>7</v>
       </c>
-      <c r="H20" s="9">
-        <v>496012</v>
-      </c>
-      <c r="I20" s="9">
-        <v>150242</v>
-      </c>
-      <c r="J20" s="9">
-        <v>370068</v>
-      </c>
-      <c r="K20" s="10">
-        <v>237637</v>
-      </c>
-      <c r="M20" s="11">
-        <f t="shared" si="1"/>
-        <v>535845.80000000005</v>
-      </c>
-      <c r="N20" s="11">
-        <f t="shared" si="0"/>
-        <v>156615.4</v>
-      </c>
-      <c r="O20" s="11">
-        <f t="shared" si="0"/>
-        <v>391896.8</v>
-      </c>
-      <c r="P20" s="11">
-        <f t="shared" si="0"/>
-        <v>243401.60000000001</v>
+      <c r="H21" s="9">
+        <v>419611</v>
+      </c>
+      <c r="I21" s="9">
+        <v>154778</v>
+      </c>
+      <c r="J21" s="9">
+        <v>379992</v>
+      </c>
+      <c r="K21" s="10">
+        <v>220263</v>
+      </c>
+      <c r="M21" s="3">
+        <v>7</v>
+      </c>
+      <c r="N21" s="9">
+        <f>AVERAGE(B9,H9,N9,B21,H21)</f>
+        <v>476111.8</v>
+      </c>
+      <c r="O21" s="9">
+        <f>AVERAGE(C9,I9,O9,C21,I21)</f>
+        <v>160325</v>
+      </c>
+      <c r="P21" s="9">
+        <f>AVERAGE(D9,J9,P9,D21,J21)</f>
+        <v>388768</v>
+      </c>
+      <c r="Q21" s="10">
+        <f>AVERAGE(E9,K9,Q9,E21,K21)</f>
+        <v>224570.2</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="6">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
         <v>8</v>
       </c>
-      <c r="B21" s="7">
-        <v>589109</v>
-      </c>
-      <c r="C21" s="7">
-        <v>184756</v>
-      </c>
-      <c r="D21" s="7">
-        <v>468271</v>
-      </c>
-      <c r="E21" s="8">
-        <v>312532</v>
-      </c>
-      <c r="G21" s="6">
+      <c r="B22" s="7">
+        <v>463854</v>
+      </c>
+      <c r="C22" s="7">
+        <v>159026</v>
+      </c>
+      <c r="D22" s="7">
+        <v>390116</v>
+      </c>
+      <c r="E22" s="8">
+        <v>224932</v>
+      </c>
+      <c r="G22" s="6">
         <v>8</v>
       </c>
-      <c r="H21" s="7">
-        <v>519126</v>
-      </c>
-      <c r="I21" s="7">
-        <v>161404</v>
-      </c>
-      <c r="J21" s="7">
-        <v>374877</v>
-      </c>
-      <c r="K21" s="8">
-        <v>239530</v>
-      </c>
-      <c r="M21" s="11">
-        <f t="shared" si="1"/>
-        <v>514118.40000000002</v>
-      </c>
-      <c r="N21" s="11">
-        <f t="shared" si="0"/>
-        <v>162147.6</v>
-      </c>
-      <c r="O21" s="11">
-        <f t="shared" si="0"/>
-        <v>388658.8</v>
-      </c>
-      <c r="P21" s="11">
-        <f t="shared" si="0"/>
-        <v>253121.4</v>
+      <c r="H22" s="7">
+        <v>448126</v>
+      </c>
+      <c r="I22" s="7">
+        <v>154400</v>
+      </c>
+      <c r="J22" s="7">
+        <v>384468</v>
+      </c>
+      <c r="K22" s="8">
+        <v>220194</v>
+      </c>
+      <c r="M22" s="6">
+        <v>8</v>
+      </c>
+      <c r="N22" s="7">
+        <f>AVERAGE(B10,H10,N10,B22,H22)</f>
+        <v>447571</v>
+      </c>
+      <c r="O22" s="7">
+        <f>AVERAGE(C10,I10,O10,C22,I22)</f>
+        <v>157352</v>
+      </c>
+      <c r="P22" s="7">
+        <f>AVERAGE(D10,J10,P10,D22,J22)</f>
+        <v>385133</v>
+      </c>
+      <c r="Q22" s="8">
+        <f>AVERAGE(E10,K10,Q10,E22,K22)</f>
+        <v>220667</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
         <v>9</v>
       </c>
-      <c r="B22" s="9">
-        <v>682737</v>
-      </c>
-      <c r="C22" s="9">
-        <v>243271</v>
-      </c>
-      <c r="D22" s="9">
-        <v>530131</v>
-      </c>
-      <c r="E22" s="10">
-        <v>288807</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="B23" s="9">
+        <v>445281</v>
+      </c>
+      <c r="C23" s="9">
+        <v>156177</v>
+      </c>
+      <c r="D23" s="9">
+        <v>391220</v>
+      </c>
+      <c r="E23" s="10">
+        <v>220375</v>
+      </c>
+      <c r="G23" s="3">
         <v>9</v>
       </c>
-      <c r="H22" s="9">
-        <v>496059</v>
-      </c>
-      <c r="I22" s="9">
-        <v>148456</v>
-      </c>
-      <c r="J22" s="9">
-        <v>389933</v>
-      </c>
-      <c r="K22" s="10">
-        <v>252656</v>
-      </c>
-      <c r="M22" s="11">
-        <f t="shared" si="1"/>
-        <v>535451.4</v>
-      </c>
-      <c r="N22" s="11">
-        <f t="shared" si="0"/>
-        <v>169716.2</v>
-      </c>
-      <c r="O22" s="11">
-        <f t="shared" si="0"/>
-        <v>408977.2</v>
-      </c>
-      <c r="P22" s="11">
-        <f t="shared" si="0"/>
-        <v>253599.6</v>
+      <c r="H23" s="9">
+        <v>425691</v>
+      </c>
+      <c r="I23" s="9">
+        <v>152134</v>
+      </c>
+      <c r="J23" s="9">
+        <v>378881</v>
+      </c>
+      <c r="K23" s="10">
+        <v>217570</v>
+      </c>
+      <c r="M23" s="3">
+        <v>9</v>
+      </c>
+      <c r="N23" s="9">
+        <f>AVERAGE(B11,H11,N11,B23,H23)</f>
+        <v>430224.8</v>
+      </c>
+      <c r="O23" s="9">
+        <f>AVERAGE(C11,I11,O11,C23,I23)</f>
+        <v>159571.4</v>
+      </c>
+      <c r="P23" s="9">
+        <f>AVERAGE(D11,J11,P11,D23,J23)</f>
+        <v>393380.2</v>
+      </c>
+      <c r="Q23" s="10">
+        <f>AVERAGE(E11,K11,Q11,E23,K23)</f>
+        <v>228973.6</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="6">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
         <v>10</v>
       </c>
-      <c r="B23" s="7">
-        <v>679609</v>
-      </c>
-      <c r="C23" s="7">
-        <v>188526</v>
-      </c>
-      <c r="D23" s="7">
-        <v>507739</v>
-      </c>
-      <c r="E23" s="8">
-        <v>308777</v>
-      </c>
-      <c r="G23" s="6">
+      <c r="B24" s="7">
+        <v>431164</v>
+      </c>
+      <c r="C24" s="7">
+        <v>157086</v>
+      </c>
+      <c r="D24" s="7">
+        <v>378163</v>
+      </c>
+      <c r="E24" s="8">
+        <v>215310</v>
+      </c>
+      <c r="G24" s="6">
         <v>10</v>
       </c>
-      <c r="H23" s="7">
-        <v>514840</v>
-      </c>
-      <c r="I23" s="7">
-        <v>154179</v>
-      </c>
-      <c r="J23" s="7">
-        <v>388205</v>
-      </c>
-      <c r="K23" s="8">
-        <v>237582</v>
-      </c>
-      <c r="M23" s="11">
-        <f t="shared" si="1"/>
-        <v>536359.4</v>
-      </c>
-      <c r="N23" s="11">
-        <f t="shared" si="0"/>
-        <v>160198.39999999999</v>
-      </c>
-      <c r="O23" s="11">
-        <f t="shared" si="0"/>
-        <v>399977.2</v>
-      </c>
-      <c r="P23" s="11">
-        <f t="shared" si="0"/>
-        <v>252373</v>
+      <c r="H24" s="7">
+        <v>420691</v>
+      </c>
+      <c r="I24" s="7">
+        <v>155951</v>
+      </c>
+      <c r="J24" s="7">
+        <v>379004</v>
+      </c>
+      <c r="K24" s="8">
+        <v>218939</v>
+      </c>
+      <c r="M24" s="6">
+        <v>10</v>
+      </c>
+      <c r="N24" s="7">
+        <f>AVERAGE(B12,H12,N12,B24,H24)</f>
+        <v>478714.4</v>
+      </c>
+      <c r="O24" s="7">
+        <f>AVERAGE(C12,I12,O12,C24,I24)</f>
+        <v>157407</v>
+      </c>
+      <c r="P24" s="7">
+        <f>AVERAGE(D12,J12,P12,D24,J24)</f>
+        <v>389241.2</v>
+      </c>
+      <c r="Q24" s="8">
+        <f>AVERAGE(E12,K12,Q12,E24,K24)</f>
+        <v>233385.8</v>
       </c>
     </row>
   </sheetData>
@@ -2814,7 +2911,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>